<commit_message>
Collation temp. Tabelle, Table Variable; Releaseplan ProjektDoku ergänzt
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjektMappe.xlsx
+++ b/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjektMappe.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85783CF-235A-41F9-8CDE-E24B81395BC7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F3562B-0335-47AA-BDBC-61CB00F1F63D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>SAXESS Software GmbH</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Gruppierungen korrigiert</t>
   </si>
   <si>
-    <t>……………….</t>
-  </si>
-  <si>
     <t>…………………………………</t>
   </si>
   <si>
@@ -140,6 +137,12 @@
   </si>
   <si>
     <t>Neue Corporate Design-Objekte</t>
+  </si>
+  <si>
+    <t>Objekt für Funktionen im Corporate Design ergänzen</t>
+  </si>
+  <si>
+    <t>Status-Farbe für deaktivert ergänzen</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,31 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -747,6 +774,536 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2776758</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Gruppieren 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B33F91-824B-414A-88AB-6FAC52DE883A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13849350" y="9153525"/>
+          <a:ext cx="1624233" cy="476250"/>
+          <a:chOff x="4747846" y="2847975"/>
+          <a:chExt cx="1620000" cy="476250"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Rechteck: abgerundete Ecken 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36505322-9868-49D0-A242-DADDF4850FB6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4747846" y="3048578"/>
+            <a:ext cx="1620000" cy="275647"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="15875">
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="de-DE" sz="900" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="69B42E"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>dbo.sx_pf_pProtectID</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="69B42E"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Textfeld 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{708473E6-FAB4-4041-8AB0-07DC3A9BA9A1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4943108" y="2883647"/>
+            <a:ext cx="1181100" cy="122590"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="de-DE" sz="900" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="69B42E"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>DataFactory</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="900" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="900" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="69B42E"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Funktion</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Rechteck 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECE5AD0-85A3-44AE-8046-3DC20859B880}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4771659" y="2847975"/>
+            <a:ext cx="122726" cy="168519"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="de-DE" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="69B42E"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>F</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>112572</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>95844</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="9" name="Gruppieren 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BB6684D-4B92-48FA-B13E-15837FAB6523}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13849350" y="9725025"/>
+          <a:ext cx="2341422" cy="743544"/>
+          <a:chOff x="1733550" y="3286125"/>
+          <a:chExt cx="2340000" cy="743544"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="10" name="Gruppieren 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C13BB4-8516-4D70-9D7C-706E1E3973A9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1733550" y="3286125"/>
+            <a:ext cx="2340000" cy="743544"/>
+            <a:chOff x="7953375" y="9620250"/>
+            <a:chExt cx="2340000" cy="743544"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="Textfeld 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8690112-D684-4AA0-8781-C946000CFF8F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8143875" y="9667875"/>
+              <a:ext cx="1181100" cy="152400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:alpha val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900">
+                  <a:solidFill>
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Prozedur </a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="Rechteck 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D86178F8-5025-4BB9-A5F7-52A177306617}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7962900" y="9620250"/>
+              <a:ext cx="122726" cy="168519"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="203864"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>P</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="Textfeld 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{973E8EFB-B48D-4801-A54F-8CFC39AD5412}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7953375" y="9823794"/>
+              <a:ext cx="2340000" cy="540000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:alpha val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="1">
+                  <a:solidFill>
+                    <a:srgbClr val="203864"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>staging.spVerrechnungssätze</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Ellipse 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97B8C53F-16CD-44D0-8814-425FA890B8F7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3829050" y="3381375"/>
+            <a:ext cx="180000" cy="180000"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1020,9 +1577,9 @@
   <dimension ref="A1:BB313"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1156,7 +1713,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
@@ -1604,7 +2161,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H30" s="37"/>
       <c r="I30" s="20">
@@ -1674,7 +2231,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H35" s="37"/>
       <c r="I35" s="20">
@@ -1696,7 +2253,7 @@
     <row r="36" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B36" s="17"/>
       <c r="C36" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H36" s="37"/>
       <c r="I36" s="20"/>
@@ -1708,7 +2265,7 @@
     </row>
     <row r="37" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C37" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H37" s="37"/>
       <c r="I37" s="20"/>
@@ -1828,7 +2385,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="I48" s="20">
         <v>0</v>
@@ -1847,13 +2404,13 @@
         <v>1</v>
       </c>
       <c r="N48" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B49" s="17"/>
       <c r="C49" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -1883,14 +2440,32 @@
       <c r="N51" s="36"/>
     </row>
     <row r="52" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="17"/>
-      <c r="C52" s="19"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="22"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="36"/>
+      <c r="B52" s="18">
+        <v>2</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="37"/>
+      <c r="I52" s="20">
+        <v>0</v>
+      </c>
+      <c r="J52" s="20">
+        <v>100</v>
+      </c>
+      <c r="K52" s="20">
+        <f>I52/100*(100-J52)</f>
+        <v>0</v>
+      </c>
+      <c r="L52" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="M52" s="22">
+        <v>1</v>
+      </c>
+      <c r="N52" s="36" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="53" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B53" s="17"/>
@@ -3580,6 +4155,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M9:M10 M16 M22:M23 M53 M33:M34 M56:M1003 M44:M50 M39:M42">
+    <cfRule type="cellIs" dxfId="23" priority="35" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="36" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M43">
     <cfRule type="cellIs" dxfId="21" priority="33" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3587,15 +4170,15 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M43">
-    <cfRule type="cellIs" dxfId="19" priority="31" operator="greaterThan">
+  <conditionalFormatting sqref="M11:M15">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M15">
+  <conditionalFormatting sqref="M17:M21">
     <cfRule type="cellIs" dxfId="17" priority="25" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3603,7 +4186,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17:M21">
+  <conditionalFormatting sqref="M51">
     <cfRule type="cellIs" dxfId="15" priority="23" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3611,7 +4194,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M51:M52">
+  <conditionalFormatting sqref="M54:M55">
     <cfRule type="cellIs" dxfId="13" priority="21" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3619,15 +4202,15 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M54:M55">
-    <cfRule type="cellIs" dxfId="11" priority="19" operator="greaterThan">
+  <conditionalFormatting sqref="M29">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M29">
+  <conditionalFormatting sqref="M24:M28">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3635,7 +4218,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:M28">
+  <conditionalFormatting sqref="M30:M32">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3643,7 +4226,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M30:M32">
+  <conditionalFormatting sqref="M38">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3651,7 +4234,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M38">
+  <conditionalFormatting sqref="M35:M37">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -3659,7 +4242,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M35:M37">
+  <conditionalFormatting sqref="M52">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Aufnahme Objekte Corporate Design
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjektMappe.xlsx
+++ b/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjektMappe.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F3562B-0335-47AA-BDBC-61CB00F1F63D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168E94BA-3049-44B3-9DAD-4770F4C3DFCE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>SAXESS Software GmbH</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Status-Farbe für deaktivert ergänzen</t>
+  </si>
+  <si>
+    <t>Grupp. Vers. für Prozessschritt manuelle u. automatisch in Corporate Design ergänzen</t>
+  </si>
+  <si>
+    <t>Objekt "Template" in Corporate Design aufnehmen</t>
   </si>
 </sst>
 </file>
@@ -358,7 +364,175 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1304,6 +1478,1027 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2555448</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>75759</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="Gruppieren 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C754E29-17A0-4013-81FF-AADC1C69DA08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13096875" y="10553700"/>
+          <a:ext cx="2155398" cy="847284"/>
+          <a:chOff x="7267575" y="22393275"/>
+          <a:chExt cx="2155398" cy="847284"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="16" name="Gruppieren 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FBCC9C3-6E39-4BFA-9B03-DE2C2B63C8AD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="7267575" y="22440900"/>
+            <a:ext cx="2124000" cy="799659"/>
+            <a:chOff x="615812" y="11645349"/>
+            <a:chExt cx="2124000" cy="799659"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="Rechteck 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97271C66-52DA-41AB-9B9A-A7160E366C4A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="615812" y="11905008"/>
+              <a:ext cx="2124000" cy="540000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Neuanlage</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>xxxxxxxxxxxxxxxxxxxxxxxxxxxxx</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1100" b="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="20" name="Grafik 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DF76A78-E74F-49F3-89B5-96695D781875}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+              <a:extLst>
+                <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                  <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                    <a14:imgLayer r:embed="rId4">
+                      <a14:imgEffect>
+                        <a14:backgroundRemoval t="0" b="100000" l="0" r="100000">
+                          <a14:foregroundMark x1="42222" y1="45333" x2="59556" y2="52889"/>
+                          <a14:foregroundMark x1="72444" y1="43556" x2="92889" y2="52444"/>
+                          <a14:foregroundMark x1="79556" y1="40000" x2="92444" y2="40444"/>
+                          <a14:foregroundMark x1="95111" y1="41778" x2="97778" y2="47556"/>
+                          <a14:foregroundMark x1="78222" y1="59111" x2="87111" y2="59111"/>
+                        </a14:backgroundRemoval>
+                      </a14:imgEffect>
+                    </a14:imgLayer>
+                  </a14:imgProps>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="646044" y="11645349"/>
+              <a:ext cx="314739" cy="314739"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="21" name="Textfeld 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0283246-0930-4429-A054-95958753D749}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1018761" y="11728174"/>
+              <a:ext cx="866775" cy="174550"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Prozessschritt</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="17" name="Grafik 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E66677B-FBF3-4EE1-AC70-F66D8C736B12}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+            <a:extLst>
+              <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a14:imgLayer r:embed="rId6">
+                    <a14:imgEffect>
+                      <a14:backgroundRemoval t="0" b="100000" l="0" r="100000">
+                        <a14:foregroundMark x1="45117" y1="36133" x2="55664" y2="33594"/>
+                        <a14:foregroundMark x1="39648" y1="29492" x2="47852" y2="19922"/>
+                        <a14:foregroundMark x1="31055" y1="18945" x2="31055" y2="18945"/>
+                        <a14:foregroundMark x1="16016" y1="40430" x2="16016" y2="40430"/>
+                        <a14:foregroundMark x1="87109" y1="52344" x2="87109" y2="52344"/>
+                      </a14:backgroundRemoval>
+                    </a14:imgEffect>
+                  </a14:imgLayer>
+                </a14:imgProps>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9117207" y="22421070"/>
+            <a:ext cx="261452" cy="273327"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="Ellipse 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAE8D517-28A2-4192-BFE6-AB7C4E6B2B58}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9077325" y="22393275"/>
+            <a:ext cx="345648" cy="347449"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2647950</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>85284</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="22" name="Gruppieren 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66E6DFE8-485C-497B-B521-4A472B582387}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="15344775" y="10353675"/>
+          <a:ext cx="2228849" cy="1056834"/>
+          <a:chOff x="9915525" y="22193250"/>
+          <a:chExt cx="2228849" cy="1056834"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="23" name="Gruppieren 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEB53D26-B1CA-41CA-BF97-03B4AB224AC3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="9915525" y="22450425"/>
+            <a:ext cx="2124000" cy="799659"/>
+            <a:chOff x="615812" y="11645349"/>
+            <a:chExt cx="2124000" cy="799659"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="27" name="Rechteck 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7B9833B-63AB-4A66-9266-4DC8C2EC6510}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="615812" y="11905008"/>
+              <a:ext cx="2124000" cy="540000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Neuanlage</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>xxxxxxxxxxxxxxxxxxxxxxxxxxxxx</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1100" b="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="28" name="Grafik 27">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD422AEA-DA63-40BF-96CE-5F00B1642D66}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+              <a:extLst>
+                <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                  <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                    <a14:imgLayer r:embed="rId4">
+                      <a14:imgEffect>
+                        <a14:backgroundRemoval t="0" b="100000" l="0" r="100000">
+                          <a14:foregroundMark x1="42222" y1="45333" x2="59556" y2="52889"/>
+                          <a14:foregroundMark x1="72444" y1="43556" x2="92889" y2="52444"/>
+                          <a14:foregroundMark x1="79556" y1="40000" x2="92444" y2="40444"/>
+                          <a14:foregroundMark x1="95111" y1="41778" x2="97778" y2="47556"/>
+                          <a14:foregroundMark x1="78222" y1="59111" x2="87111" y2="59111"/>
+                        </a14:backgroundRemoval>
+                      </a14:imgEffect>
+                    </a14:imgLayer>
+                  </a14:imgProps>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="646044" y="11645349"/>
+              <a:ext cx="314739" cy="314739"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="29" name="Textfeld 28">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4CBAAA4-5026-409C-97D8-E61FBBAC8A09}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1018761" y="11728174"/>
+              <a:ext cx="866775" cy="174550"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Prozessschritt</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="24" name="Gruppieren 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5292A201-357B-49EB-928B-93EC844E8731}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="11220450" y="22193250"/>
+            <a:ext cx="923924" cy="485776"/>
+            <a:chOff x="5505451" y="371475"/>
+            <a:chExt cx="923924" cy="485776"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="25" name="Rechteck: abgerundete Ecken 24">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A61389DD-71F7-4F62-87EF-A03FECE8299F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5505451" y="552451"/>
+              <a:ext cx="819149" cy="304800"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="800">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>täglich</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="800" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t> 12:00</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="800">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="26" name="Grafik 25">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78BD659C-4EEA-407E-BFA2-BDBF57319D75}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+              <a:extLst>
+                <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                  <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                    <a14:imgLayer r:embed="rId8">
+                      <a14:imgEffect>
+                        <a14:backgroundRemoval t="1125" b="99375" l="1500" r="100000">
+                          <a14:foregroundMark x1="19375" y1="33875" x2="19375" y2="33875"/>
+                          <a14:foregroundMark x1="30750" y1="22250" x2="30750" y2="22250"/>
+                          <a14:foregroundMark x1="36375" y1="21625" x2="36375" y2="21625"/>
+                          <a14:foregroundMark x1="48000" y1="17125" x2="48000" y2="17125"/>
+                          <a14:foregroundMark x1="53250" y1="16500" x2="53250" y2="16500"/>
+                          <a14:foregroundMark x1="69125" y1="19125" x2="69125" y2="19125"/>
+                          <a14:foregroundMark x1="83750" y1="30250" x2="83750" y2="30250"/>
+                          <a14:foregroundMark x1="88250" y1="46250" x2="88250" y2="46250"/>
+                          <a14:foregroundMark x1="82750" y1="64750" x2="82750" y2="64750"/>
+                          <a14:foregroundMark x1="67250" y1="77375" x2="67250" y2="77375"/>
+                          <a14:foregroundMark x1="51750" y1="81125" x2="51750" y2="81125"/>
+                          <a14:foregroundMark x1="35625" y1="77125" x2="35625" y2="77125"/>
+                          <a14:foregroundMark x1="18375" y1="65375" x2="18375" y2="65375"/>
+                          <a14:foregroundMark x1="16125" y1="49250" x2="16125" y2="49250"/>
+                          <a14:foregroundMark x1="22500" y1="34125" x2="22500" y2="34125"/>
+                          <a14:foregroundMark x1="29250" y1="87750" x2="29250" y2="87750"/>
+                          <a14:foregroundMark x1="30125" y1="92625" x2="30125" y2="92625"/>
+                          <a14:foregroundMark x1="51000" y1="93000" x2="51000" y2="93000"/>
+                          <a14:foregroundMark x1="72625" y1="86875" x2="72625" y2="86875"/>
+                          <a14:foregroundMark x1="88250" y1="71375" x2="88250" y2="71375"/>
+                          <a14:foregroundMark x1="93750" y1="49750" x2="93750" y2="49750"/>
+                          <a14:foregroundMark x1="87750" y1="28750" x2="87750" y2="28750"/>
+                          <a14:foregroundMark x1="72250" y1="12750" x2="72250" y2="12750"/>
+                          <a14:foregroundMark x1="50750" y1="7000" x2="50750" y2="7000"/>
+                          <a14:foregroundMark x1="29750" y1="12625" x2="29750" y2="12625"/>
+                          <a14:foregroundMark x1="13500" y1="28625" x2="13500" y2="28625"/>
+                          <a14:foregroundMark x1="7375" y1="50250" x2="7375" y2="50250"/>
+                          <a14:foregroundMark x1="13375" y1="71500" x2="13375" y2="71500"/>
+                        </a14:backgroundRemoval>
+                      </a14:imgEffect>
+                    </a14:imgLayer>
+                  </a14:imgProps>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6172200" y="371475"/>
+              <a:ext cx="257175" cy="257175"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2258175</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>186510</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="30" name="Gruppieren 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C75DB749-F71A-4AE4-BEAA-7D501DB1D3CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13335000" y="11496675"/>
+          <a:ext cx="1620000" cy="777060"/>
+          <a:chOff x="5838824" y="5791794"/>
+          <a:chExt cx="1620000" cy="777060"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="31" name="Rechteck: abgerundete Ecken 30">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CFF0805-DA92-4D9C-9F4F-C33D8AB070A2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5838824" y="6028854"/>
+            <a:ext cx="1620000" cy="540000"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="15875">
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="de-DE" sz="900" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="69B42E"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Konto</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="de-DE" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="69B42E"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Info</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="32" name="Grafik 31">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3CD7A6E-01D9-482B-8B54-997EEE2B43DE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5887810" y="5791794"/>
+            <a:ext cx="172686" cy="166215"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="33" name="Textfeld 32">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D0FCA10-4AB4-4C71-9C68-281B5459902E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6162675" y="5822429"/>
+            <a:ext cx="866775" cy="165025"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="de-DE" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="69B42E"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Template</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="34" name="Grafik 33">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4A70BB9-9643-4C04-A662-53E4B0EEF76D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5915025" y="5830966"/>
+            <a:ext cx="170089" cy="163715"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="35" name="Ellipse 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19936A33-A754-4F8B-A53C-E1BCE40A2706}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7124700" y="5943600"/>
+            <a:ext cx="180000" cy="180000"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1579,7 +2774,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomLeft" activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2400,9 +3595,7 @@
       <c r="L48" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M48" s="22">
-        <v>1</v>
-      </c>
+      <c r="M48" s="22"/>
       <c r="N48" s="36" t="s">
         <v>33</v>
       </c>
@@ -2460,9 +3653,7 @@
       <c r="L52" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M52" s="22">
-        <v>1</v>
-      </c>
+      <c r="M52" s="22"/>
       <c r="N52" s="36" t="s">
         <v>33</v>
       </c>
@@ -2498,60 +3689,118 @@
       <c r="N55" s="36"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="23"/>
-      <c r="M56" s="23"/>
+      <c r="B56" s="18">
+        <v>3</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H56" s="37"/>
+      <c r="I56" s="20">
+        <v>0</v>
+      </c>
+      <c r="J56" s="20">
+        <v>100</v>
+      </c>
+      <c r="K56" s="20">
+        <f>I56/100*(100-J56)</f>
+        <v>0</v>
+      </c>
+      <c r="L56" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="M56" s="22"/>
+      <c r="N56" s="36"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="23"/>
-      <c r="M57" s="23"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="19"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="22"/>
+      <c r="M57" s="22"/>
+      <c r="N57" s="36"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
-      <c r="L58" s="23"/>
-      <c r="M58" s="23"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="11"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="22"/>
+      <c r="N58" s="36"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I59" s="21"/>
-      <c r="J59" s="21"/>
-      <c r="K59" s="21"/>
-      <c r="L59" s="23"/>
-      <c r="M59" s="23"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="22"/>
+      <c r="N59" s="36"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I60" s="21"/>
-      <c r="J60" s="21"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="23"/>
-      <c r="M60" s="23"/>
+      <c r="B60" s="18">
+        <v>4</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H60" s="37"/>
+      <c r="I60" s="20">
+        <v>0</v>
+      </c>
+      <c r="J60" s="20">
+        <v>100</v>
+      </c>
+      <c r="K60" s="20">
+        <f>I60/100*(100-J60)</f>
+        <v>0</v>
+      </c>
+      <c r="L60" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="M60" s="22"/>
+      <c r="N60" s="36"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I61" s="21"/>
-      <c r="J61" s="21"/>
-      <c r="K61" s="21"/>
-      <c r="L61" s="23"/>
-      <c r="M61" s="23"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="19"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="36"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I62" s="21"/>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="23"/>
-      <c r="M62" s="23"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="11"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+      <c r="N62" s="36"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I63" s="21"/>
-      <c r="J63" s="21"/>
-      <c r="K63" s="21"/>
-      <c r="L63" s="23"/>
-      <c r="M63" s="23"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="36"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I64" s="21"/>
@@ -4154,55 +5403,103 @@
       <c r="K313" s="21"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M9:M10 M16 M22:M23 M53 M33:M34 M56:M1003 M44:M50 M39:M42">
-    <cfRule type="cellIs" dxfId="23" priority="35" operator="greaterThan">
+  <conditionalFormatting sqref="M9:M10 M16 M22:M23 M53 M33:M34 M44:M50 M39:M42 M64:M1003">
+    <cfRule type="cellIs" dxfId="37" priority="49" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M43">
-    <cfRule type="cellIs" dxfId="21" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="47" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11:M15">
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="41" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17:M21">
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M51">
-    <cfRule type="cellIs" dxfId="15" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="37" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:M55">
-    <cfRule type="cellIs" dxfId="13" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="35" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M24:M28">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M30:M32">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M38">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M35:M37">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M52">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M56">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -4210,7 +5507,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:M28">
+  <conditionalFormatting sqref="M60">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -4218,7 +5515,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M30:M32">
+  <conditionalFormatting sqref="M57">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -4226,7 +5523,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M38">
+  <conditionalFormatting sqref="M58:M59">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -4234,7 +5531,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M35:M37">
+  <conditionalFormatting sqref="M61">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -4242,7 +5539,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M52">
+  <conditionalFormatting sqref="M62:M63">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Punkte in Releaseplan ergänzt
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjektMappe.xlsx
+++ b/8. Harmonising standards/01_Project organisation/03_Project Documentation/ReleasePlan_Template ProjektMappe.xlsx
@@ -3,14 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168E94BA-3049-44B3-9DAD-4770F4C3DFCE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E5FB39-F29F-4A38-A51B-1FDE7FE7CA7E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4725" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleasePlan" sheetId="46" r:id="rId1"/>
+    <sheet name="5" sheetId="47" r:id="rId2"/>
+    <sheet name="6" sheetId="48" r:id="rId3"/>
+    <sheet name="7" sheetId="49" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>SAXESS Software GmbH</t>
   </si>
@@ -150,12 +153,30 @@
   <si>
     <t>Objekt "Template" in Corporate Design aufnehmen</t>
   </si>
+  <si>
+    <t>Formel in Abrechnung korrekt auf alle Zeilen kopieren</t>
+  </si>
+  <si>
+    <t>Button Drucken verbessern</t>
+  </si>
+  <si>
+    <t>1. umbennen in "Speichern als pdf"</t>
+  </si>
+  <si>
+    <t>2. bei Abbrechen wirklich abbrechen</t>
+  </si>
+  <si>
+    <t>Dropdown Box für Status definieren</t>
+  </si>
+  <si>
+    <t>Vorgeschlagen, geplant, Auftrag avisiert, beauftragt, in Arbeit, erledigt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +243,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -272,10 +301,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -360,35 +390,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <font>
         <b/>
@@ -2502,6 +2510,171 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28514</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A09C7299-2739-42C0-A1D1-DD0C38CA403F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1095375" y="1047750"/>
+          <a:ext cx="10058400" cy="3552764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>277540</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95768</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4446B5F4-BE52-4084-B178-EC3B5582F132}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="762000"/>
+          <a:ext cx="9421540" cy="3715268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>112080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D72F22B-3AAA-4489-A0D3-2BD1B8052917}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="381000"/>
+          <a:ext cx="10058400" cy="5065080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2772,9 +2945,9 @@
   <dimension ref="A1:BB313"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H33" sqref="H33"/>
-      <selection pane="bottomLeft" activeCell="N60" sqref="N60"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3781,8 +3954,12 @@
       <c r="N61" s="36"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="18"/>
-      <c r="C62" s="11"/>
+      <c r="B62" s="18">
+        <v>5</v>
+      </c>
+      <c r="C62" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H62" s="37"/>
       <c r="I62" s="20"/>
       <c r="J62" s="20"/>
@@ -3803,118 +3980,139 @@
       <c r="N63" s="36"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B64" s="18">
+        <v>6</v>
+      </c>
+      <c r="C64" s="38" t="s">
+        <v>44</v>
+      </c>
       <c r="I64" s="21"/>
       <c r="J64" s="21"/>
       <c r="K64" s="21"/>
       <c r="L64" s="23"/>
       <c r="M64" s="23"/>
     </row>
-    <row r="65" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C65" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="I65" s="21"/>
       <c r="J65" s="21"/>
       <c r="K65" s="21"/>
       <c r="L65" s="23"/>
       <c r="M65" s="23"/>
     </row>
-    <row r="66" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C66" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="I66" s="21"/>
       <c r="J66" s="21"/>
       <c r="K66" s="21"/>
       <c r="L66" s="23"/>
       <c r="M66" s="23"/>
     </row>
-    <row r="67" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I67" s="21"/>
       <c r="J67" s="21"/>
       <c r="K67" s="21"/>
       <c r="L67" s="23"/>
       <c r="M67" s="23"/>
     </row>
-    <row r="68" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B68" s="18">
+        <v>7</v>
+      </c>
+      <c r="C68" s="38" t="s">
+        <v>47</v>
+      </c>
       <c r="I68" s="21"/>
       <c r="J68" s="21"/>
       <c r="K68" s="21"/>
       <c r="L68" s="23"/>
       <c r="M68" s="23"/>
     </row>
-    <row r="69" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C69" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="I69" s="21"/>
       <c r="J69" s="21"/>
       <c r="K69" s="21"/>
       <c r="L69" s="23"/>
       <c r="M69" s="23"/>
     </row>
-    <row r="70" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I70" s="21"/>
       <c r="J70" s="21"/>
       <c r="K70" s="21"/>
       <c r="L70" s="23"/>
       <c r="M70" s="23"/>
     </row>
-    <row r="71" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I71" s="21"/>
       <c r="J71" s="21"/>
       <c r="K71" s="21"/>
       <c r="L71" s="23"/>
       <c r="M71" s="23"/>
     </row>
-    <row r="72" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I72" s="21"/>
       <c r="J72" s="21"/>
       <c r="K72" s="21"/>
       <c r="L72" s="23"/>
       <c r="M72" s="23"/>
     </row>
-    <row r="73" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I73" s="21"/>
       <c r="J73" s="21"/>
       <c r="K73" s="21"/>
       <c r="L73" s="23"/>
       <c r="M73" s="23"/>
     </row>
-    <row r="74" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I74" s="21"/>
       <c r="J74" s="21"/>
       <c r="K74" s="21"/>
       <c r="L74" s="23"/>
       <c r="M74" s="23"/>
     </row>
-    <row r="75" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I75" s="21"/>
       <c r="J75" s="21"/>
       <c r="K75" s="21"/>
       <c r="L75" s="23"/>
       <c r="M75" s="23"/>
     </row>
-    <row r="76" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I76" s="21"/>
       <c r="J76" s="21"/>
       <c r="K76" s="21"/>
       <c r="L76" s="23"/>
       <c r="M76" s="23"/>
     </row>
-    <row r="77" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I77" s="21"/>
       <c r="J77" s="21"/>
       <c r="K77" s="21"/>
       <c r="L77" s="23"/>
       <c r="M77" s="23"/>
     </row>
-    <row r="78" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I78" s="21"/>
       <c r="J78" s="21"/>
       <c r="K78" s="21"/>
       <c r="L78" s="23"/>
       <c r="M78" s="23"/>
     </row>
-    <row r="79" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I79" s="21"/>
       <c r="J79" s="21"/>
       <c r="K79" s="21"/>
       <c r="L79" s="23"/>
       <c r="M79" s="23"/>
     </row>
-    <row r="80" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I80" s="21"/>
       <c r="J80" s="21"/>
       <c r="K80" s="21"/>
@@ -5404,98 +5602,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M9:M10 M16 M22:M23 M53 M33:M34 M44:M50 M39:M42 M64:M1003">
-    <cfRule type="cellIs" dxfId="37" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="49" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M43">
-    <cfRule type="cellIs" dxfId="35" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="47" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11:M15">
-    <cfRule type="cellIs" dxfId="33" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="41" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17:M21">
-    <cfRule type="cellIs" dxfId="31" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="39" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M51">
-    <cfRule type="cellIs" dxfId="29" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="37" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:M55">
-    <cfRule type="cellIs" dxfId="27" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="35" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24:M28">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30:M32">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M38">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M35:M37">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5547,8 +5745,64 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C62" location="'5'!A1" display="Formel in Abrechnung korrekt auf alle Zeilen kopieren" xr:uid="{EE86D39E-B8DB-472F-9DB0-460676CF9C3F}"/>
+    <hyperlink ref="C64" location="'6'!A1" display="Button Drucken verbessern" xr:uid="{6AAB1971-04DB-4A04-941C-B88A27E2F5E0}"/>
+    <hyperlink ref="C68" location="'7'!A1" display="Dropdown Box für Status definieren" xr:uid="{7D74A72B-62D7-43EA-8E49-6F0B651A117F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1654065-DC76-4895-BC57-B8863C25B740}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3840E2A7-AE74-4A47-8711-A90CCEA055E0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F86857F-34B8-4496-9D2F-06809D925CC6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>